<commit_message>
Adjusted readme, uploaded mob programming photo, and updated sprint burndown chart.
</commit_message>
<xml_diff>
--- a/Team Burndown Chart - Team Rosetta.xlsx
+++ b/Team Burndown Chart - Team Rosetta.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuacoffie/Google Drive/School Documents/Harvard University Extension School/Harvard University - Summer 2016/Agile Software Development/Team Project Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuacoffie/Google Drive/School Documents/Harvard University Extension School/Harvard University - Summer 2016/Team Github Folder/team_rosetta/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Team Rosetta Sprint Planning" sheetId="1" r:id="rId1"/>
@@ -218,21 +218,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -297,6 +288,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,7 +488,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6.0</c:v>
@@ -621,28 +615,28 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>9.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>21.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>27.0</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41.0</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41.0</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -798,28 +792,28 @@
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>44.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>32.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>26.0</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>26.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,11 +829,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2080811408"/>
-        <c:axId val="-2080913456"/>
+        <c:axId val="-2134061344"/>
+        <c:axId val="-2144854624"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2080811408"/>
+        <c:axId val="-2134061344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,14 +876,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080913456"/>
+        <c:crossAx val="-2144854624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2080913456"/>
+        <c:axId val="-2144854624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080811408"/>
+        <c:crossAx val="-2134061344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1159,7 +1153,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.0</c:v>
@@ -1244,25 +1238,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>9.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>21.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>27.0</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.0</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1379,25 +1373,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>32.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>26.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.0</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1412,11 +1406,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2140764384"/>
-        <c:axId val="-2063112208"/>
+        <c:axId val="-2134257040"/>
+        <c:axId val="-2134264656"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2140764384"/>
+        <c:axId val="-2134257040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,14 +1453,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063112208"/>
+        <c:crossAx val="-2134264656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2063112208"/>
+        <c:axId val="-2134264656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1516,7 +1510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140764384"/>
+        <c:crossAx val="-2134257040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3026,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="149" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="149" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3069,46 +3063,46 @@
       <c r="B4" s="1">
         <v>53</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>42545</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>0</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>0</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="18">
         <f>E4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="11">
         <f>B4-E4</f>
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>42546</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>3</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="13">
         <f>F4+E5</f>
         <v>3</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="19">
         <f>E5+H4</f>
         <v>3</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="14">
         <f>I4-E5</f>
         <v>50</v>
       </c>
@@ -3117,24 +3111,24 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>42547</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <v>0</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="13">
         <f t="shared" ref="F6:F16" si="0">F5+E6</f>
         <v>3</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="19">
         <f t="shared" ref="H6:H17" si="1">E6+H5</f>
         <v>3</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="14">
         <f t="shared" ref="I6:I17" si="2">I5-E6</f>
         <v>50</v>
       </c>
@@ -3143,271 +3137,271 @@
       <c r="B7" s="1">
         <v>38</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>42548</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>0</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="14">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>42549</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <v>0</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="14">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>42550</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="20">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="17">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="24">
         <v>42551</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G10" s="11">
+        <f>B7-E10</f>
+        <v>38</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="22"/>
+      <c r="D11" s="3">
+        <v>42552</v>
+      </c>
+      <c r="E11" s="4">
         <v>6</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G10" s="5">
-        <f>B7-E10</f>
+      <c r="G11" s="5">
+        <f>G10-E11</f>
         <v>32</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H11" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I11" s="5">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C11" s="25"/>
-      <c r="D11" s="6">
-        <v>42552</v>
-      </c>
-      <c r="E11" s="7">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="22"/>
+      <c r="D12" s="3">
+        <v>42553</v>
+      </c>
+      <c r="E12" s="4">
         <v>6</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G11" s="8">
-        <f>G10-E11</f>
+      <c r="G12" s="5">
+        <f t="shared" ref="G12:G16" si="3">G11-E12</f>
         <v>26</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H12" s="4">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I12" s="5">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C12" s="25"/>
-      <c r="D12" s="6">
-        <v>42553</v>
-      </c>
-      <c r="E12" s="7">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="22"/>
+      <c r="D13" s="3">
+        <v>42554</v>
+      </c>
+      <c r="E13" s="4">
         <v>6</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F13" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G12" s="8">
-        <f t="shared" ref="G12:G16" si="3">G11-E12</f>
+      <c r="G13" s="5">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H13" s="4">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I13" s="5">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="25"/>
-      <c r="D13" s="6">
-        <v>42554</v>
-      </c>
-      <c r="E13" s="7">
-        <v>6</v>
-      </c>
-      <c r="F13" s="7">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C14" s="22"/>
+      <c r="D14" s="3">
+        <v>42555</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="G13" s="8">
+        <v>21</v>
+      </c>
+      <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="H13" s="7">
+        <v>20</v>
+      </c>
+      <c r="H14" s="4">
         <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="I13" s="8">
+        <v>21</v>
+      </c>
+      <c r="I14" s="5">
         <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C14" s="25"/>
-      <c r="D14" s="6">
-        <v>42555</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="G14" s="8">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="H14" s="7">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="I14" s="8">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C15" s="25"/>
-      <c r="D15" s="6">
+      <c r="C15" s="22"/>
+      <c r="D15" s="3">
         <v>42556</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="4">
         <v>7</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="G15" s="8">
+        <v>28</v>
+      </c>
+      <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="H15" s="7">
+        <v>13</v>
+      </c>
+      <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="I15" s="8">
+        <v>28</v>
+      </c>
+      <c r="I15" s="5">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C16" s="26"/>
-      <c r="D16" s="9">
+      <c r="C16" s="23"/>
+      <c r="D16" s="6">
         <v>42557</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="7">
         <v>7</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="G16" s="11">
+        <v>35</v>
+      </c>
+      <c r="G16" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="10">
+        <v>6</v>
+      </c>
+      <c r="H16" s="7">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="I16" s="11">
+        <v>35</v>
+      </c>
+      <c r="I16" s="8">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <v>42558</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="16">
         <v>0</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="16">
         <v>0</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="16">
         <v>0</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="16">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="I17" s="20">
+        <v>35</v>
+      </c>
+      <c r="I17" s="17">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Pair Programming evidence and updated burndown chart.
</commit_message>
<xml_diff>
--- a/Team Burndown Chart - Team Rosetta.xlsx
+++ b/Team Burndown Chart - Team Rosetta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="460" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="3620" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Team Rosetta Sprint Planning" sheetId="1" r:id="rId1"/>
@@ -280,6 +280,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -288,9 +291,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,22 +491,22 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.0</c:v>
@@ -618,25 +618,25 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -795,25 +795,25 @@
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,11 +829,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2134061344"/>
-        <c:axId val="-2144854624"/>
+        <c:axId val="2115789872"/>
+        <c:axId val="2075706096"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2134061344"/>
+        <c:axId val="2115789872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,14 +876,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144854624"/>
+        <c:crossAx val="2075706096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2144854624"/>
+        <c:axId val="2075706096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134061344"/>
+        <c:crossAx val="2115789872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1156,22 +1156,22 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1241,22 +1241,22 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1376,22 +1376,22 @@
                   <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1406,11 +1406,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2134257040"/>
-        <c:axId val="-2134264656"/>
+        <c:axId val="2116579664"/>
+        <c:axId val="2116582736"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2134257040"/>
+        <c:axId val="2116579664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,14 +1453,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134264656"/>
+        <c:crossAx val="2116582736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2134264656"/>
+        <c:axId val="2116582736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,7 +1510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134257040"/>
+        <c:crossAx val="2116579664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3020,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="149" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3206,10 +3206,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>42551</v>
       </c>
       <c r="E10" s="10">
@@ -3233,82 +3233,82 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="3">
         <v>42552</v>
       </c>
       <c r="E11" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G11" s="5">
         <f>G10-E11</f>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C12" s="22"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="3">
         <v>42553</v>
       </c>
       <c r="E12" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" ref="G12:G16" si="3">G11-E12</f>
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="22"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="3">
         <v>42554</v>
       </c>
       <c r="E13" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C14" s="22"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="3">
         <v>42555</v>
       </c>
@@ -3317,69 +3317,69 @@
       </c>
       <c r="F14" s="4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C15" s="22"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="3">
         <v>42556</v>
       </c>
       <c r="E15" s="4">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C16" s="23"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="6">
         <v>42557</v>
       </c>
       <c r="E16" s="7">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I16" s="8">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.2">
@@ -3397,11 +3397,11 @@
       </c>
       <c r="H17" s="16">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I17" s="17">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final update to API branch
</commit_message>
<xml_diff>
--- a/Team Burndown Chart - Team Rosetta.xlsx
+++ b/Team Burndown Chart - Team Rosetta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="3620" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="27880" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Team Rosetta Sprint Planning" sheetId="1" r:id="rId1"/>
@@ -829,11 +829,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2115789872"/>
-        <c:axId val="2075706096"/>
+        <c:axId val="2098230208"/>
+        <c:axId val="2098226992"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2115789872"/>
+        <c:axId val="2098230208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,14 +876,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2075706096"/>
+        <c:crossAx val="2098226992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2075706096"/>
+        <c:axId val="2098226992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115789872"/>
+        <c:crossAx val="2098230208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1302,8 +1302,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.467224448545124"/>
-                  <c:y val="-0.151968242428307"/>
+                  <c:x val="0.0577307076697016"/>
+                  <c:y val="0.195158857349812"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1406,11 +1406,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2116579664"/>
-        <c:axId val="2116582736"/>
+        <c:axId val="2100610896"/>
+        <c:axId val="2100613968"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2116579664"/>
+        <c:axId val="2100610896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,14 +1453,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2116582736"/>
+        <c:crossAx val="2100613968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2116582736"/>
+        <c:axId val="2100613968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,7 +1510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2116579664"/>
+        <c:crossAx val="2100610896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3020,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="149" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="149" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Converging documents to this branch for team submission.
</commit_message>
<xml_diff>
--- a/Team Burndown Chart - Team Rosetta.xlsx
+++ b/Team Burndown Chart - Team Rosetta.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuacoffie/Google Drive/School Documents/Harvard University Extension School/Harvard University - Summer 2016/Agile Software Development/Team Project Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuacoffie/Google Drive/School Documents/Harvard University Extension School/Harvard University - Summer 2016/Team Github Folder/team_rosetta/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="27880" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Team Rosetta Sprint Planning" sheetId="1" r:id="rId1"/>
@@ -218,21 +218,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -287,6 +278,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -494,25 +488,25 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.0</c:v>
@@ -621,22 +615,22 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>41.0</c:v>
@@ -798,22 +792,22 @@
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>12.0</c:v>
@@ -835,11 +829,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2080811408"/>
-        <c:axId val="-2080913456"/>
+        <c:axId val="2098230208"/>
+        <c:axId val="2098226992"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2080811408"/>
+        <c:axId val="2098230208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,14 +876,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080913456"/>
+        <c:crossAx val="2098226992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2080913456"/>
+        <c:axId val="2098226992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080811408"/>
+        <c:crossAx val="2098230208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1159,25 +1153,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,22 +1238,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>41.0</c:v>
@@ -1308,8 +1302,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.467224448545124"/>
-                  <c:y val="-0.151968242428307"/>
+                  <c:x val="0.0577307076697016"/>
+                  <c:y val="0.195158857349812"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1379,22 +1373,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>32.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -1412,11 +1406,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2140764384"/>
-        <c:axId val="-2063112208"/>
+        <c:axId val="2100610896"/>
+        <c:axId val="2100613968"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2140764384"/>
+        <c:axId val="2100610896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,14 +1453,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063112208"/>
+        <c:crossAx val="2100613968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2063112208"/>
+        <c:axId val="2100613968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1516,7 +1510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140764384"/>
+        <c:crossAx val="2100610896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3026,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="149" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="149" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3069,46 +3063,46 @@
       <c r="B4" s="1">
         <v>53</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>42545</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>0</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>0</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="18">
         <f>E4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="11">
         <f>B4-E4</f>
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>42546</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>3</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="13">
         <f>F4+E5</f>
         <v>3</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="19">
         <f>E5+H4</f>
         <v>3</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="14">
         <f>I4-E5</f>
         <v>50</v>
       </c>
@@ -3117,24 +3111,24 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>42547</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <v>0</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="13">
         <f t="shared" ref="F6:F16" si="0">F5+E6</f>
         <v>3</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="19">
         <f t="shared" ref="H6:H17" si="1">E6+H5</f>
         <v>3</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="14">
         <f t="shared" ref="I6:I17" si="2">I5-E6</f>
         <v>50</v>
       </c>
@@ -3143,269 +3137,269 @@
       <c r="B7" s="1">
         <v>38</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>42548</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>0</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="14">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>42549</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <v>0</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="14">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>42550</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="20">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="17">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="21">
         <v>42551</v>
       </c>
-      <c r="E10" s="4">
-        <v>6</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G10" s="5">
+        <v>3</v>
+      </c>
+      <c r="G10" s="11">
         <f>B7-E10</f>
-        <v>32</v>
-      </c>
-      <c r="H10" s="4">
+        <v>38</v>
+      </c>
+      <c r="H10" s="10">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="I10" s="5">
+        <v>3</v>
+      </c>
+      <c r="I10" s="11">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C11" s="25"/>
-      <c r="D11" s="6">
+      <c r="C11" s="23"/>
+      <c r="D11" s="3">
         <v>42552</v>
       </c>
-      <c r="E11" s="7">
-        <v>6</v>
-      </c>
-      <c r="F11" s="7">
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="G11" s="8">
+        <v>3</v>
+      </c>
+      <c r="G11" s="5">
         <f>G10-E11</f>
-        <v>26</v>
-      </c>
-      <c r="H11" s="7">
+        <v>38</v>
+      </c>
+      <c r="H11" s="4">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="I11" s="8">
+        <v>3</v>
+      </c>
+      <c r="I11" s="5">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C12" s="25"/>
-      <c r="D12" s="6">
+      <c r="C12" s="23"/>
+      <c r="D12" s="3">
         <v>42553</v>
       </c>
-      <c r="E12" s="7">
-        <v>6</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="G12" s="8">
+        <v>3</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" ref="G12:G16" si="3">G11-E12</f>
-        <v>20</v>
-      </c>
-      <c r="H12" s="7">
+        <v>38</v>
+      </c>
+      <c r="H12" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="I12" s="8">
+        <v>3</v>
+      </c>
+      <c r="I12" s="5">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="25"/>
-      <c r="D13" s="6">
+      <c r="C13" s="23"/>
+      <c r="D13" s="3">
         <v>42554</v>
       </c>
-      <c r="E13" s="7">
-        <v>6</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="G13" s="8">
+        <v>3</v>
+      </c>
+      <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="H13" s="7">
+        <v>38</v>
+      </c>
+      <c r="H13" s="4">
         <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="I13" s="8">
+        <v>3</v>
+      </c>
+      <c r="I13" s="5">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C14" s="25"/>
-      <c r="D14" s="6">
+      <c r="C14" s="23"/>
+      <c r="D14" s="3">
         <v>42555</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="4">
         <v>0</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="4">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="G14" s="8">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="H14" s="7">
+        <v>38</v>
+      </c>
+      <c r="H14" s="4">
         <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="I14" s="8">
+        <v>3</v>
+      </c>
+      <c r="I14" s="5">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C15" s="25"/>
-      <c r="D15" s="6">
+      <c r="C15" s="23"/>
+      <c r="D15" s="3">
         <v>42556</v>
       </c>
-      <c r="E15" s="7">
-        <v>7</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="E15" s="4">
+        <v>17</v>
+      </c>
+      <c r="F15" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="G15" s="8">
+        <v>20</v>
+      </c>
+      <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="H15" s="7">
+        <v>21</v>
+      </c>
+      <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="I15" s="8">
+        <v>20</v>
+      </c>
+      <c r="I15" s="5">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C16" s="26"/>
-      <c r="D16" s="9">
+      <c r="C16" s="24"/>
+      <c r="D16" s="6">
         <v>42557</v>
       </c>
-      <c r="E16" s="10">
-        <v>7</v>
-      </c>
-      <c r="F16" s="10">
+      <c r="E16" s="7">
+        <v>21</v>
+      </c>
+      <c r="F16" s="7">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="7">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="8">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <v>42558</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="16">
         <v>0</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="16">
         <v>0</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="16">
         <v>0</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="16">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="17">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>

</xml_diff>